<commit_message>
adding forecast and updated excel spreadsheet
</commit_message>
<xml_diff>
--- a/proj1/ResidentialCustomerForecastLoad-624.xlsx
+++ b/proj1/ResidentialCustomerForecastLoad-624.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\my project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="4752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="4752" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ResidentialCustomerForecastLoad" sheetId="1" r:id="rId1"/>
+    <sheet name="ResidentialCustomerForecastLoad" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="KWH-2014-Forecast" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
   <si>
     <t>CaseSequence</t>
   </si>
@@ -604,13 +599,59 @@
   </si>
   <si>
     <t>2013-Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaseSequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YYYY-MMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KWH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Apr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Jun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Jul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Aug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Sep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Oct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Dec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -637,20 +678,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -990,2141 +1023,2299 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C193"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>733</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1" t="n">
         <v>6862583</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>734</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1" t="n">
         <v>5838198</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>735</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1" t="n">
         <v>5420658</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>736</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1" t="n">
         <v>5010364</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>737</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1" t="n">
         <v>4665377</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>738</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1" t="n">
         <v>6467147</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>739</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1" t="n">
         <v>8914755</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>740</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1" t="n">
         <v>8607428</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>741</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1" t="n">
         <v>6989888</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>742</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1" t="n">
         <v>6345620</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>743</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1" t="n">
         <v>4640410</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13">
+      <c r="A13" s="1" t="n">
         <v>744</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="1" t="n">
         <v>4693479</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14">
+      <c r="A14" s="1" t="n">
         <v>745</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="1" t="n">
         <v>7183759</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>746</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1" t="n">
         <v>5759262</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>747</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1" t="n">
         <v>4847656</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17">
+      <c r="A17" s="1" t="n">
         <v>748</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1" t="n">
         <v>5306592</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18">
+      <c r="A18" s="1" t="n">
         <v>749</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="1" t="n">
         <v>4426794</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19">
+      <c r="A19" s="1" t="n">
         <v>750</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1" t="n">
         <v>5500901</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20">
+      <c r="A20" s="1" t="n">
         <v>751</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1" t="n">
         <v>7444416</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21">
+      <c r="A21" s="1" t="n">
         <v>752</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="1" t="n">
         <v>7564391</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>753</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="1" t="n">
         <v>7899368</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23">
+      <c r="A23" s="1" t="n">
         <v>754</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="1" t="n">
         <v>5358314</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24">
+      <c r="A24" s="1" t="n">
         <v>755</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="1" t="n">
         <v>4436269</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25">
+      <c r="A25" s="1" t="n">
         <v>756</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="1" t="n">
         <v>4419229</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="26">
+      <c r="A26" s="1" t="n">
         <v>757</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="1" t="n">
         <v>7068296</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27">
+      <c r="A27" s="1" t="n">
         <v>758</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="1" t="n">
         <v>5876083</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28">
+      <c r="A28" s="1" t="n">
         <v>759</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="1" t="n">
         <v>4807961</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="29">
+      <c r="A29" s="1" t="n">
         <v>760</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="1" t="n">
         <v>4873080</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="30">
+      <c r="A30" s="1" t="n">
         <v>761</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="1" t="n">
         <v>5050891</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31">
+      <c r="A31" s="1" t="n">
         <v>762</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="1" t="n">
         <v>7092865</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="32">
+      <c r="A32" s="1" t="n">
         <v>763</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="1" t="n">
         <v>6862662</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33">
+      <c r="A33" s="1" t="n">
         <v>764</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="1" t="n">
         <v>7517830</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="34">
+      <c r="A34" s="1" t="n">
         <v>765</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="1" t="n">
         <v>8912169</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35">
+      <c r="A35" s="1" t="n">
         <v>766</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="1" t="n">
         <v>5844352</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36">
+      <c r="A36" s="1" t="n">
         <v>767</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="1" t="n">
         <v>5041769</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="37">
+      <c r="A37" s="1" t="n">
         <v>768</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="1" t="n">
         <v>6220334</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="38">
+      <c r="A38" s="1" t="n">
         <v>769</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="1" t="n">
         <v>7538529</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="39">
+      <c r="A39" s="1" t="n">
         <v>770</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="1" t="n">
         <v>6602448</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="40">
+      <c r="A40" s="1" t="n">
         <v>771</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="1" t="n">
         <v>5779180</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="41">
+      <c r="A41" s="1" t="n">
         <v>772</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="1" t="n">
         <v>4835210</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="42">
+      <c r="A42" s="1" t="n">
         <v>773</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="1" t="n">
         <v>4787904</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="43">
+      <c r="A43" s="1" t="n">
         <v>774</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="1" t="n">
         <v>6283324</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="44">
+      <c r="A44" s="1" t="n">
         <v>775</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="1" t="n">
         <v>7855129</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="45">
+      <c r="A45" s="1" t="n">
         <v>776</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="1" t="n">
         <v>8450717</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="46">
+      <c r="A46" s="1" t="n">
         <v>777</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="1" t="n">
         <v>7112069</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+    <row r="47">
+      <c r="A47" s="1" t="n">
         <v>778</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="1" t="n">
         <v>5242535</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="48">
+      <c r="A48" s="1" t="n">
         <v>779</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="1" t="n">
         <v>4461979</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+    <row r="49">
+      <c r="A49" s="1" t="n">
         <v>780</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="1" t="n">
         <v>5240995</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    <row r="50">
+      <c r="A50" s="1" t="n">
         <v>781</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="1" t="n">
         <v>7099063</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+    <row r="51">
+      <c r="A51" s="1" t="n">
         <v>782</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="1" t="n">
         <v>6413429</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+    <row r="52">
+      <c r="A52" s="1" t="n">
         <v>783</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="1" t="n">
         <v>5839514</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+    <row r="53">
+      <c r="A53" s="1" t="n">
         <v>784</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="1" t="n">
         <v>5371604</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+    <row r="54">
+      <c r="A54" s="1" t="n">
         <v>785</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="1" t="n">
         <v>5439166</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="55">
+      <c r="A55" s="1" t="n">
         <v>786</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="1" t="n">
         <v>5850383</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+    <row r="56">
+      <c r="A56" s="1" t="n">
         <v>787</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="1" t="n">
         <v>7039702</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+    <row r="57">
+      <c r="A57" s="1" t="n">
         <v>788</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="1" t="n">
         <v>8058748</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+    <row r="58">
+      <c r="A58" s="1" t="n">
         <v>789</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="1" t="n">
         <v>8245227</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+    <row r="59">
+      <c r="A59" s="1" t="n">
         <v>790</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="1" t="n">
         <v>5865014</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+    <row r="60">
+      <c r="A60" s="1" t="n">
         <v>791</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="1" t="n">
         <v>4908979</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+    <row r="61">
+      <c r="A61" s="1" t="n">
         <v>792</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="1" t="n">
         <v>5779958</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+    <row r="62">
+      <c r="A62" s="1" t="n">
         <v>793</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="1" t="n">
         <v>7256079</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+    <row r="63">
+      <c r="A63" s="1" t="n">
         <v>794</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="1" t="n">
         <v>6190517</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+    <row r="64">
+      <c r="A64" s="1" t="n">
         <v>795</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="1" t="n">
         <v>6120626</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+    <row r="65">
+      <c r="A65" s="1" t="n">
         <v>796</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="1" t="n">
         <v>4885643</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+    <row r="66">
+      <c r="A66" s="1" t="n">
         <v>797</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="1" t="n">
         <v>5296096</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+    <row r="67">
+      <c r="A67" s="1" t="n">
         <v>798</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="1" t="n">
         <v>6051571</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+    <row r="68">
+      <c r="A68" s="1" t="n">
         <v>799</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="1" t="n">
         <v>6900676</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+    <row r="69">
+      <c r="A69" s="1" t="n">
         <v>800</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="1" t="n">
         <v>8476499</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+    <row r="70">
+      <c r="A70" s="1" t="n">
         <v>801</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="1" t="n">
         <v>7791791</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+    <row r="71">
+      <c r="A71" s="1" t="n">
         <v>802</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="1" t="n">
         <v>5344613</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+    <row r="72">
+      <c r="A72" s="1" t="n">
         <v>803</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="1" t="n">
         <v>4913707</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+    <row r="73">
+      <c r="A73" s="1" t="n">
         <v>804</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="1" t="n">
         <v>5756193</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+    <row r="74">
+      <c r="A74" s="1" t="n">
         <v>805</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="1" t="n">
         <v>7584596</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+    <row r="75">
+      <c r="A75" s="1" t="n">
         <v>806</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="1" t="n">
         <v>6560742</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+    <row r="76">
+      <c r="A76" s="1" t="n">
         <v>807</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="1" t="n">
         <v>6526586</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+    <row r="77">
+      <c r="A77" s="1" t="n">
         <v>808</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="1" t="n">
         <v>4831688</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+    <row r="78">
+      <c r="A78" s="1" t="n">
         <v>809</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="1" t="n">
         <v>4878262</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+    <row r="79">
+      <c r="A79" s="1" t="n">
         <v>810</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="1" t="n">
         <v>6421614</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+    <row r="80">
+      <c r="A80" s="1" t="n">
         <v>811</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="1" t="n">
         <v>7307931</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+    <row r="81">
+      <c r="A81" s="1" t="n">
         <v>812</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="1" t="n">
         <v>7309774</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+    <row r="82">
+      <c r="A82" s="1" t="n">
         <v>813</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="1" t="n">
         <v>6690366</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>814</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="1" t="n">
         <v>5444948</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+    <row r="84">
+      <c r="A84" s="1" t="n">
         <v>815</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="1" t="n">
         <v>4824940</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+    <row r="85">
+      <c r="A85" s="1" t="n">
         <v>816</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="1" t="n">
         <v>5791208</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+    <row r="86">
+      <c r="A86" s="1" t="n">
         <v>817</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="1" t="n">
         <v>8225477</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+    <row r="87">
+      <c r="A87" s="1" t="n">
         <v>818</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="1" t="n">
         <v>6564338</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+    <row r="88">
+      <c r="A88" s="1" t="n">
         <v>819</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="1" t="n">
         <v>5581725</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="89">
+      <c r="A89" s="1" t="n">
         <v>820</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="1" t="n">
         <v>5563071</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+    <row r="90">
+      <c r="A90" s="1" t="n">
         <v>821</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="1" t="n">
         <v>4453983</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+    <row r="91">
+      <c r="A91" s="1" t="n">
         <v>822</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="1" t="n">
         <v>5900212</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+    <row r="92">
+      <c r="A92" s="1" t="n">
         <v>823</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92" s="1" t="n">
         <v>8337998</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+    <row r="93">
+      <c r="A93" s="1" t="n">
         <v>824</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93" s="1" t="n">
         <v>7786659</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="94">
+      <c r="A94" s="1" t="n">
         <v>825</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94" s="1" t="n">
         <v>7057213</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+    <row r="95">
+      <c r="A95" s="1" t="n">
         <v>826</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95" s="1" t="n">
         <v>6694523</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+    <row r="96">
+      <c r="A96" s="1" t="n">
         <v>827</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96" s="1" t="n">
         <v>4313019</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+    <row r="97">
+      <c r="A97" s="1" t="n">
         <v>828</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97" s="1" t="n">
         <v>6181548</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+    <row r="98">
+      <c r="A98" s="1" t="n">
         <v>829</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="1" t="n">
         <v>7793358</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+    <row r="99">
+      <c r="A99" s="1" t="n">
         <v>830</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="1" t="n">
         <v>5914945</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+    <row r="100">
+      <c r="A100" s="1" t="n">
         <v>831</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="1" t="n">
         <v>5819734</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+    <row r="101">
+      <c r="A101" s="1" t="n">
         <v>832</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="1" t="n">
         <v>5255988</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+    <row r="102">
+      <c r="A102" s="1" t="n">
         <v>833</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="1" t="n">
         <v>4740588</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+    <row r="103">
+      <c r="A103" s="1" t="n">
         <v>834</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="1" t="n">
         <v>7052275</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+    <row r="104">
+      <c r="A104" s="1" t="n">
         <v>835</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C104" s="1" t="n">
         <v>7945564</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+    <row r="105">
+      <c r="A105" s="1" t="n">
         <v>836</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C105" s="3">
+      <c r="C105" s="1" t="n">
         <v>8241110</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+    <row r="106">
+      <c r="A106" s="1" t="n">
         <v>837</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C106" s="1" t="n">
         <v>7296355</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+    <row r="107">
+      <c r="A107" s="1" t="n">
         <v>838</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C107" s="1" t="n">
         <v>5104799</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+    <row r="108">
+      <c r="A108" s="1" t="n">
         <v>839</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C108" s="3">
+      <c r="C108" s="1" t="n">
         <v>4458429</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+    <row r="109">
+      <c r="A109" s="1" t="n">
         <v>840</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C109" s="3">
+      <c r="C109" s="1" t="n">
         <v>6226214</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+    <row r="110">
+      <c r="A110" s="1" t="n">
         <v>841</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C110" s="3">
+      <c r="C110" s="1" t="n">
         <v>8031295</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+    <row r="111">
+      <c r="A111" s="1" t="n">
         <v>842</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C111" s="3">
+      <c r="C111" s="1" t="n">
         <v>7928337</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+    <row r="112">
+      <c r="A112" s="1" t="n">
         <v>843</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C112" s="3">
+      <c r="C112" s="1" t="n">
         <v>6443170</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+    <row r="113">
+      <c r="A113" s="1" t="n">
         <v>844</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C113" s="3">
+      <c r="C113" s="1" t="n">
         <v>4841979</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+    <row r="114">
+      <c r="A114" s="1" t="n">
         <v>845</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C114" s="1" t="n">
         <v>4862847</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+    <row r="115">
+      <c r="A115" s="1" t="n">
         <v>846</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C115" s="1" t="n">
         <v>5022647</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+    <row r="116">
+      <c r="A116" s="1" t="n">
         <v>847</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C116" s="3">
+      <c r="C116" s="1" t="n">
         <v>6426220</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+    <row r="117">
+      <c r="A117" s="1" t="n">
         <v>848</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C117" s="3">
+      <c r="C117" s="1" t="n">
         <v>7447146</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+    <row r="118">
+      <c r="A118" s="1" t="n">
         <v>849</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C118" s="3">
+      <c r="C118" s="1" t="n">
         <v>7666970</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+    <row r="119">
+      <c r="A119" s="1" t="n">
         <v>850</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C119" s="3">
+      <c r="C119" s="1" t="n">
         <v>5785964</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
+    <row r="120">
+      <c r="A120" s="1" t="n">
         <v>851</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C120" s="3">
+      <c r="C120" s="1" t="n">
         <v>4907057</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+    <row r="121">
+      <c r="A121" s="1" t="n">
         <v>852</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C121" s="3">
+      <c r="C121" s="1" t="n">
         <v>6047292</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
+    <row r="122">
+      <c r="A122" s="1" t="n">
         <v>853</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C122" s="3">
+      <c r="C122" s="1" t="n">
         <v>7964293</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+    <row r="123">
+      <c r="A123" s="1" t="n">
         <v>854</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C123" s="3">
+      <c r="C123" s="1" t="n">
         <v>7597060</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
+    <row r="124">
+      <c r="A124" s="1" t="n">
         <v>855</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C124" s="3">
+      <c r="C124" s="1" t="n">
         <v>6085644</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
+    <row r="125">
+      <c r="A125" s="1" t="n">
         <v>856</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C125" s="3">
+      <c r="C125" s="1" t="n">
         <v>5352359</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+    <row r="126">
+      <c r="A126" s="1" t="n">
         <v>857</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C126" s="3">
+      <c r="C126" s="1" t="n">
         <v>4608528</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+    <row r="127">
+      <c r="A127" s="1" t="n">
         <v>858</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C127" s="3">
+      <c r="C127" s="1" t="n">
         <v>6548439</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
+    <row r="128">
+      <c r="A128" s="1" t="n">
         <v>859</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C128" s="3">
+      <c r="C128" s="1" t="n">
         <v>7643987</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
+    <row r="129">
+      <c r="A129" s="1" t="n">
         <v>860</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C129" s="3">
+      <c r="C129" s="1" t="n">
         <v>8037137</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
+    <row r="130">
+      <c r="A130" s="1" t="n">
         <v>861</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
+    <row r="131">
+      <c r="A131" s="1" t="n">
         <v>862</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C131" s="3">
+      <c r="C131" s="1" t="n">
         <v>5101803</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
+    <row r="132">
+      <c r="A132" s="1" t="n">
         <v>863</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C132" s="3">
+      <c r="C132" s="1" t="n">
         <v>4555602</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
+    <row r="133">
+      <c r="A133" s="1" t="n">
         <v>864</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C133" s="3">
+      <c r="C133" s="1" t="n">
         <v>6442746</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
+    <row r="134">
+      <c r="A134" s="1" t="n">
         <v>865</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C134" s="3">
+      <c r="C134" s="1" t="n">
         <v>8072330</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
+    <row r="135">
+      <c r="A135" s="1" t="n">
         <v>866</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C135" s="3">
+      <c r="C135" s="1" t="n">
         <v>6976800</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
+    <row r="136">
+      <c r="A136" s="1" t="n">
         <v>867</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C136" s="3">
+      <c r="C136" s="1" t="n">
         <v>5691452</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
+    <row r="137">
+      <c r="A137" s="1" t="n">
         <v>868</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C137" s="3">
+      <c r="C137" s="1" t="n">
         <v>5531616</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
+    <row r="138">
+      <c r="A138" s="1" t="n">
         <v>869</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C138" s="3">
+      <c r="C138" s="1" t="n">
         <v>5264439</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
+    <row r="139">
+      <c r="A139" s="1" t="n">
         <v>870</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C139" s="3">
+      <c r="C139" s="1" t="n">
         <v>5804433</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
+    <row r="140">
+      <c r="A140" s="1" t="n">
         <v>871</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C140" s="3">
+      <c r="C140" s="1" t="n">
         <v>7713260</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
+    <row r="141">
+      <c r="A141" s="1" t="n">
         <v>872</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C141" s="3">
+      <c r="C141" s="1" t="n">
         <v>8350517</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
+    <row r="142">
+      <c r="A142" s="1" t="n">
         <v>873</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C142" s="3">
+      <c r="C142" s="1" t="n">
         <v>7583146</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+    <row r="143">
+      <c r="A143" s="1" t="n">
         <v>874</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C143" s="3">
+      <c r="C143" s="1" t="n">
         <v>5566075</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
+    <row r="144">
+      <c r="A144" s="1" t="n">
         <v>875</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B144" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C144" s="3">
+      <c r="C144" s="1" t="n">
         <v>5339890</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
+    <row r="145">
+      <c r="A145" s="1" t="n">
         <v>876</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C145" s="3">
+      <c r="C145" s="1" t="n">
         <v>7089880</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
+    <row r="146">
+      <c r="A146" s="1" t="n">
         <v>877</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C146" s="3">
+      <c r="C146" s="1" t="n">
         <v>9397357</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
+    <row r="147">
+      <c r="A147" s="1" t="n">
         <v>878</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B147" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C147" s="3">
+      <c r="C147" s="1" t="n">
         <v>8390677</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
+    <row r="148">
+      <c r="A148" s="1" t="n">
         <v>879</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B148" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C148" s="3">
+      <c r="C148" s="1" t="n">
         <v>7347915</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
+    <row r="149">
+      <c r="A149" s="1" t="n">
         <v>880</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B149" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C149" s="3">
+      <c r="C149" s="1" t="n">
         <v>5776131</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
+    <row r="150">
+      <c r="A150" s="1" t="n">
         <v>881</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B150" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C150" s="3">
+      <c r="C150" s="1" t="n">
         <v>4919289</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
+    <row r="151">
+      <c r="A151" s="1" t="n">
         <v>882</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B151" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C151" s="3">
+      <c r="C151" s="1" t="n">
         <v>6696292</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
+    <row r="152">
+      <c r="A152" s="1" t="n">
         <v>883</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C152" s="3">
+      <c r="C152" s="1" t="n">
         <v>770523</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
+    <row r="153">
+      <c r="A153" s="1" t="n">
         <v>884</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B153" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C153" s="3">
+      <c r="C153" s="1" t="n">
         <v>7922701</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
+    <row r="154">
+      <c r="A154" s="1" t="n">
         <v>885</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B154" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C154" s="3">
+      <c r="C154" s="1" t="n">
         <v>7819472</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
+    <row r="155">
+      <c r="A155" s="1" t="n">
         <v>886</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B155" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C155" s="3">
+      <c r="C155" s="1" t="n">
         <v>5875917</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
+    <row r="156">
+      <c r="A156" s="1" t="n">
         <v>887</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B156" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C156" s="3">
+      <c r="C156" s="1" t="n">
         <v>4800733</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
+    <row r="157">
+      <c r="A157" s="1" t="n">
         <v>888</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C157" s="3">
+      <c r="C157" s="1" t="n">
         <v>6152583</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
+    <row r="158">
+      <c r="A158" s="1" t="n">
         <v>889</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B158" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C158" s="3">
+      <c r="C158" s="1" t="n">
         <v>8394747</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
+    <row r="159">
+      <c r="A159" s="1" t="n">
         <v>890</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B159" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C159" s="3">
+      <c r="C159" s="1" t="n">
         <v>8898062</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
+    <row r="160">
+      <c r="A160" s="1" t="n">
         <v>891</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B160" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C160" s="3">
+      <c r="C160" s="1" t="n">
         <v>6356903</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
+    <row r="161">
+      <c r="A161" s="1" t="n">
         <v>892</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B161" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C161" s="3">
+      <c r="C161" s="1" t="n">
         <v>5685227</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
+    <row r="162">
+      <c r="A162" s="1" t="n">
         <v>893</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C162" s="3">
+      <c r="C162" s="1" t="n">
         <v>5506308</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
+    <row r="163">
+      <c r="A163" s="1" t="n">
         <v>894</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C163" s="3">
+      <c r="C163" s="1" t="n">
         <v>8037779</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
+    <row r="164">
+      <c r="A164" s="1" t="n">
         <v>895</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B164" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C164" s="3">
+      <c r="C164" s="1" t="n">
         <v>10093343</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
+    <row r="165">
+      <c r="A165" s="1" t="n">
         <v>896</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B165" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C165" s="3">
+      <c r="C165" s="1" t="n">
         <v>10308076</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
+    <row r="166">
+      <c r="A166" s="1" t="n">
         <v>897</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B166" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C166" s="3">
+      <c r="C166" s="1" t="n">
         <v>8943599</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
+    <row r="167">
+      <c r="A167" s="1" t="n">
         <v>898</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B167" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C167" s="3">
+      <c r="C167" s="1" t="n">
         <v>5603920</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
+    <row r="168">
+      <c r="A168" s="1" t="n">
         <v>899</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B168" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C168" s="3">
+      <c r="C168" s="1" t="n">
         <v>6154138</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
+    <row r="169">
+      <c r="A169" s="1" t="n">
         <v>900</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B169" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C169" s="3">
+      <c r="C169" s="1" t="n">
         <v>8273142</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
+    <row r="170">
+      <c r="A170" s="1" t="n">
         <v>901</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B170" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C170" s="3">
+      <c r="C170" s="1" t="n">
         <v>8991267</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
+    <row r="171">
+      <c r="A171" s="1" t="n">
         <v>902</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B171" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C171" s="3">
+      <c r="C171" s="1" t="n">
         <v>7952204</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
+    <row r="172">
+      <c r="A172" s="1" t="n">
         <v>903</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C172" s="3">
+      <c r="C172" s="1" t="n">
         <v>6356961</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
+    <row r="173">
+      <c r="A173" s="1" t="n">
         <v>904</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C173" s="3">
+      <c r="C173" s="1" t="n">
         <v>5569828</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
+    <row r="174">
+      <c r="A174" s="1" t="n">
         <v>905</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B174" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C174" s="3">
+      <c r="C174" s="1" t="n">
         <v>5783598</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
+    <row r="175">
+      <c r="A175" s="1" t="n">
         <v>906</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C175" s="3">
+      <c r="C175" s="1" t="n">
         <v>7926956</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
+    <row r="176">
+      <c r="A176" s="1" t="n">
         <v>907</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B176" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C176" s="3">
+      <c r="C176" s="1" t="n">
         <v>8886851</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
+    <row r="177">
+      <c r="A177" s="1" t="n">
         <v>908</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B177" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C177" s="3">
+      <c r="C177" s="1" t="n">
         <v>9612423</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
+    <row r="178">
+      <c r="A178" s="1" t="n">
         <v>909</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B178" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C178" s="3">
+      <c r="C178" s="1" t="n">
         <v>7559148</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
+    <row r="179">
+      <c r="A179" s="1" t="n">
         <v>910</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C179" s="3">
+      <c r="C179" s="1" t="n">
         <v>5576852</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
+    <row r="180">
+      <c r="A180" s="1" t="n">
         <v>911</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B180" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C180" s="3">
+      <c r="C180" s="1" t="n">
         <v>5731899</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
+    <row r="181">
+      <c r="A181" s="1" t="n">
         <v>912</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B181" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C181" s="3">
+      <c r="C181" s="1" t="n">
         <v>6609694</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
+    <row r="182">
+      <c r="A182" s="1" t="n">
         <v>913</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B182" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C182" s="3">
+      <c r="C182" s="1" t="n">
         <v>10655730</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
+    <row r="183">
+      <c r="A183" s="1" t="n">
         <v>914</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C183" s="3">
+      <c r="C183" s="1" t="n">
         <v>7681798</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
+    <row r="184">
+      <c r="A184" s="1" t="n">
         <v>915</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C184" s="3">
+      <c r="C184" s="1" t="n">
         <v>6517514</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
+    <row r="185">
+      <c r="A185" s="1" t="n">
         <v>916</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C185" s="3">
+      <c r="C185" s="1" t="n">
         <v>6105359</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
+    <row r="186">
+      <c r="A186" s="1" t="n">
         <v>917</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C186" s="3">
+      <c r="C186" s="1" t="n">
         <v>5940475</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
+    <row r="187">
+      <c r="A187" s="1" t="n">
         <v>918</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C187" s="3">
+      <c r="C187" s="1" t="n">
         <v>7920627</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
+    <row r="188">
+      <c r="A188" s="1" t="n">
         <v>919</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B188" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C188" s="3">
+      <c r="C188" s="1" t="n">
         <v>8415321</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
+    <row r="189">
+      <c r="A189" s="1" t="n">
         <v>920</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C189" s="3">
+      <c r="C189" s="1" t="n">
         <v>9080226</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
+    <row r="190">
+      <c r="A190" s="1" t="n">
         <v>921</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B190" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C190" s="3">
+      <c r="C190" s="1" t="n">
         <v>7968220</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
+    <row r="191">
+      <c r="A191" s="1" t="n">
         <v>922</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C191" s="3">
+      <c r="C191" s="1" t="n">
         <v>5759367</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
+    <row r="192">
+      <c r="A192" s="1" t="n">
         <v>923</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B192" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C192" s="3">
+      <c r="C192" s="1" t="n">
         <v>5769083</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
+    <row r="193">
+      <c r="A193" s="1" t="n">
         <v>924</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B193" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C193" s="3">
+      <c r="C193" s="1" t="n">
         <v>9606304</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>925</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9639577.29392796</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>926</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8751725.49250378</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>927</v>
+      </c>
+      <c r="B4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7275339.66681299</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>928</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6511576.46451415</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>929</v>
+      </c>
+      <c r="B6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6178933.65022497</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>930</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7743768.76042125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>931</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8053326.72064516</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>932</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9438396.76403724</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>933</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8569088.7593862</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>934</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6495009.69732719</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>935</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6201950.37709561</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>936</v>
+      </c>
+      <c r="B13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" t="n">
+        <v>8075443.119988</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding final edited documents
</commit_message>
<xml_diff>
--- a/proj1/ResidentialCustomerForecastLoad-624.xlsx
+++ b/proj1/ResidentialCustomerForecastLoad-624.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
   <si>
     <t>CaseSequence</t>
   </si>
@@ -644,6 +644,21 @@
   </si>
   <si>
     <t xml:space="preserve">2014-Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forecast_KWH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lo80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lo95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi95</t>
   </si>
 </sst>
 </file>
@@ -3179,7 +3194,19 @@
         <v>196</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>210</v>
+      </c>
+      <c r="D1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="2">
@@ -3190,7 +3217,19 @@
         <v>198</v>
       </c>
       <c r="C2" t="n">
-        <v>9639577.29392796</v>
+        <v>9878216.82779281</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7851527.24526238</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11904906.4103232</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6778662.58713754</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12977771.0684481</v>
       </c>
     </row>
     <row r="3">
@@ -3201,7 +3240,19 @@
         <v>199</v>
       </c>
       <c r="C3" t="n">
-        <v>8751725.49250378</v>
+        <v>7226198.35794253</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5735949.25104287</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8716447.4648422</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4947059.02711498</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9505337.68877008</v>
       </c>
     </row>
     <row r="4">
@@ -3212,7 +3263,19 @@
         <v>200</v>
       </c>
       <c r="C4" t="n">
-        <v>7275339.66681299</v>
+        <v>7138953.97698387</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5659158.897073</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8618749.05689475</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4875802.70074758</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9402105.25322017</v>
       </c>
     </row>
     <row r="5">
@@ -3223,7 +3286,19 @@
         <v>201</v>
       </c>
       <c r="C5" t="n">
-        <v>6511576.46451415</v>
+        <v>7063420.08973674</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5591859.39939538</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8534980.7800781</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4812862.22559937</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9313977.95387412</v>
       </c>
     </row>
     <row r="6">
@@ -3234,7 +3309,19 @@
         <v>202</v>
       </c>
       <c r="C6" t="n">
-        <v>6178933.65022497</v>
+        <v>7248142.56535106</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5730517.16880919</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8765767.96189294</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4927134.81254841</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9569150.31815371</v>
       </c>
     </row>
     <row r="7">
@@ -3245,7 +3332,19 @@
         <v>203</v>
       </c>
       <c r="C7" t="n">
-        <v>7743768.76042125</v>
+        <v>8797783.97566991</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6946534.87439008</v>
+      </c>
+      <c r="E7" t="n">
+        <v>10649033.0769497</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5966542.79702977</v>
+      </c>
+      <c r="G7" t="n">
+        <v>11629025.1543101</v>
       </c>
     </row>
     <row r="8">
@@ -3256,7 +3355,19 @@
         <v>204</v>
       </c>
       <c r="C8" t="n">
-        <v>8053326.72064516</v>
+        <v>7599171.48630383</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5992263.83487319</v>
+      </c>
+      <c r="E8" t="n">
+        <v>9206079.13773448</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5141618.30782714</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10056724.6647805</v>
       </c>
     </row>
     <row r="9">
@@ -3267,7 +3378,19 @@
         <v>205</v>
       </c>
       <c r="C9" t="n">
-        <v>9438396.76403724</v>
+        <v>7693797.79159447</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6058946.16913086</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9328649.41405807</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5193507.99737626</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10194087.5858127</v>
       </c>
     </row>
     <row r="10">
@@ -3278,7 +3401,19 @@
         <v>206</v>
       </c>
       <c r="C10" t="n">
-        <v>8569088.7593862</v>
+        <v>6801231.32952394</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5349058.85373009</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8253403.80531779</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4580325.1807442</v>
+      </c>
+      <c r="G10" t="n">
+        <v>9022137.47830368</v>
       </c>
     </row>
     <row r="11">
@@ -3289,7 +3424,19 @@
         <v>207</v>
       </c>
       <c r="C11" t="n">
-        <v>6495009.69732719</v>
+        <v>5116287.26016041</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4018649.07689258</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6213925.44342824</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3437594.5215294</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6794979.99879142</v>
       </c>
     </row>
     <row r="12">
@@ -3300,7 +3447,19 @@
         <v>208</v>
       </c>
       <c r="C12" t="n">
-        <v>6201950.37709561</v>
+        <v>6997840.54727104</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5489418.48843338</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8506262.6061087</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4690908.08486074</v>
+      </c>
+      <c r="G12" t="n">
+        <v>9304773.00968134</v>
       </c>
     </row>
     <row r="13">
@@ -3311,7 +3470,19 @@
         <v>209</v>
       </c>
       <c r="C13" t="n">
-        <v>8075443.119988</v>
+        <v>9152049.68401973</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7170006.94078882</v>
+      </c>
+      <c r="E13" t="n">
+        <v>11134092.4272506</v>
+      </c>
+      <c r="F13" t="n">
+        <v>6120776.89173008</v>
+      </c>
+      <c r="G13" t="n">
+        <v>12183322.4763094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>